<commit_message>
meto nombre de columnas
</commit_message>
<xml_diff>
--- a/resources/renta_por_barrios.xlsx
+++ b/resources/renta_por_barrios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FerWolowitz\Desktop\MASTER\PHYTON\Repositorio\G3_ProyectoPython\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\G3_ProyectoPython\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
   <si>
     <t xml:space="preserve"> 01. Centro</t>
   </si>
@@ -471,6 +471,12 @@
   </si>
   <si>
     <t xml:space="preserve">   215. Corralejos</t>
+  </si>
+  <si>
+    <t>DISTRITO</t>
+  </si>
+  <si>
+    <t>RENTA_MEDIA</t>
   </si>
 </sst>
 </file>
@@ -835,1283 +841,1291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B169"/>
+  <dimension ref="A1:B170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B169"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B2" s="2">
         <v>31377.836360012756</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>34675.847913459736</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>25999.832743082243</v>
+        <v>34675.847913459736</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>34952.679804656669</v>
+        <v>25999.832743082243</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>40314.882263767009</v>
+        <v>34952.679804656669</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4">
-        <v>30701.652039292203</v>
+        <v>40314.882263767009</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>30701.652039292203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B8" s="4">
         <v>30935.804311342592</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-    </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
         <v>40200.656654275088</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4">
-        <v>41950.812045864746</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="4">
-        <v>44669.182438943455</v>
+        <v>41950.812045864746</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4">
-        <v>31933.911996619991</v>
+        <v>44669.182438943455</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4">
-        <v>48935.036576627012</v>
+        <v>31933.911996619991</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="4">
-        <v>39647.688652559234</v>
+        <v>48935.036576627012</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4">
-        <v>33938.36905297661</v>
+        <v>39647.688652559234</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4">
+        <v>33938.36905297661</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B17" s="4">
         <v>37939.284722891563</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-    </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B19" s="2">
         <v>51789.996070997135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="4">
-        <v>41948.887029967016</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="4">
-        <v>45842.92865148378</v>
+        <v>41948.887029967016</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="4">
-        <v>58249.144489218801</v>
+        <v>45842.92865148378</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4">
-        <v>45561.1376637797</v>
+        <v>58249.144489218801</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="4">
-        <v>84955.30244799405</v>
+        <v>45561.1376637797</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="4">
+        <v>84955.30244799405</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B25" s="4">
         <v>69100.160909916463</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-    </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B27" s="2">
         <v>53971.852404971003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="4">
-        <v>84705.717880827317</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="4">
-        <v>48814.737832512321</v>
+        <v>84705.717880827317</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="4">
-        <v>40503.559002474132</v>
+        <v>48814.737832512321</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="4">
-        <v>46340.874098849337</v>
+        <v>40503.559002474132</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="4">
-        <v>47375.424529116586</v>
+        <v>46340.874098849337</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="4">
+        <v>47375.424529116586</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B33" s="4">
         <v>82811.17901163717</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-    </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B35" s="2">
         <v>60947.890897262136</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="4">
-        <v>103573.08265600556</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" s="4">
-        <v>43701.522001574493</v>
+        <v>103573.08265600556</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="4">
-        <v>43706.982619804076</v>
+        <v>43701.522001574493</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="4">
-        <v>62635.35035399715</v>
+        <v>43706.982619804076</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="4">
-        <v>80248.392025596288</v>
+        <v>62635.35035399715</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="4">
+        <v>80248.392025596288</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B41" s="4">
         <v>54869.965013558787</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="6"/>
-    </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="5"/>
+      <c r="B42" s="6"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B43" s="2">
         <v>34700.359566811167</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="4">
-        <v>31125.229902695948</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" s="4">
-        <v>43306.023276175816</v>
+        <v>31125.229902695948</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" s="4">
-        <v>45025.326885959883</v>
+        <v>43306.023276175816</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" s="4">
-        <v>28746.703366257949</v>
+        <v>45025.326885959883</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" s="4">
-        <v>28242.052362314509</v>
+        <v>28746.703366257949</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="4">
+        <v>28242.052362314509</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B49" s="4">
         <v>28945.525477272728</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="3"/>
-      <c r="B49" s="7"/>
-    </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="3"/>
+      <c r="B50" s="7"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B51" s="2">
         <v>48989.345061970438</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B51" s="4">
-        <v>42607.636540203282</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" s="4">
-        <v>42210.151776515151</v>
+        <v>42607.636540203282</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B53" s="4">
-        <v>41126.219802584354</v>
+        <v>42210.151776515151</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B54" s="4">
-        <v>68786.709213910755</v>
+        <v>41126.219802584354</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B55" s="4">
-        <v>47955.279166739681</v>
+        <v>68786.709213910755</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" s="4">
+        <v>47955.279166739681</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B57" s="4">
         <v>59458.575400225483</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="8"/>
-      <c r="B57" s="10"/>
-    </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="8"/>
+      <c r="B58" s="10"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B59" s="2">
         <v>48846.591040665946</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B59" s="4">
-        <v>39061.727086553321</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B60" s="4">
-        <v>98155.792942289496</v>
+        <v>39061.727086553321</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B61" s="4">
-        <v>45508.058073087683</v>
+        <v>98155.792942289496</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B62" s="4">
-        <v>33746.013818845568</v>
+        <v>45508.058073087683</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B63" s="4">
-        <v>58457.375286918461</v>
+        <v>33746.013818845568</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B64" s="4">
-        <v>42537.250096005242</v>
+        <v>58457.375286918461</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B65" s="4">
-        <v>78328.100556215562</v>
+        <v>42537.250096005242</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B66" s="4">
+        <v>78328.100556215562</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B67" s="4">
         <v>57441.344233021082</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="8"/>
-      <c r="B67" s="10"/>
-    </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="8"/>
+      <c r="B68" s="10"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B69" s="2">
         <v>56443.788702975085</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B69" s="4">
-        <v>41436.083852990181</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B70" s="4">
-        <v>53460.643562335827</v>
+        <v>41436.083852990181</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B71" s="4">
-        <v>67390.492096167014</v>
+        <v>53460.643562335827</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B72" s="4">
-        <v>34996.93079768688</v>
+        <v>67390.492096167014</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B73" s="4">
-        <v>112320.74809387521</v>
+        <v>34996.93079768688</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B74" s="4">
-        <v>101419.17171036206</v>
+        <v>112320.74809387521</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B75" s="4">
+        <v>101419.17171036206</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B75" s="4">
+      <c r="B76" s="4">
         <v>77060.755639745345</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="11"/>
-      <c r="B76" s="10"/>
-    </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="8" t="s">
+      <c r="A77" s="11"/>
+      <c r="B77" s="10"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B78" s="2">
         <v>30155.742529572341</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B78" s="4">
-        <v>29540.957694128785</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B79" s="4">
-        <v>27913.633911254252</v>
+        <v>29540.957694128785</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B80" s="4">
-        <v>30075.705553614327</v>
+        <v>27913.633911254252</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B81" s="4">
-        <v>31116.507119747333</v>
+        <v>30075.705553614327</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B82" s="4">
-        <v>31913.206846745976</v>
+        <v>31116.507119747333</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B83" s="4">
-        <v>35197.134509999996</v>
+        <v>31913.206846745976</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B84" s="4">
+        <v>35197.134509999996</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B84" s="4">
+      <c r="B85" s="4">
         <v>29910.454936174392</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="5"/>
-      <c r="B85" s="6"/>
-    </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="8" t="s">
+      <c r="A86" s="5"/>
+      <c r="B86" s="6"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B87" s="2">
         <v>27935.706747110475</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B87" s="4">
-        <v>27579.227944311508</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B88" s="4">
-        <v>28031.479104203292</v>
+        <v>27579.227944311508</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B89" s="4">
-        <v>26282.724397873222</v>
+        <v>28031.479104203292</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B90" s="4">
-        <v>27788.213282112843</v>
+        <v>26282.724397873222</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B91" s="4">
-        <v>25725.18725548061</v>
+        <v>27788.213282112843</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B92" s="4">
-        <v>31280.562009904053</v>
+        <v>25725.18725548061</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B93" s="4">
+        <v>31280.562009904053</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B93" s="4">
+      <c r="B94" s="4">
         <v>27997.611786321559</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="11"/>
-      <c r="B94" s="10"/>
-    </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="8" t="s">
+      <c r="A95" s="11"/>
+      <c r="B95" s="10"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B96" s="2">
         <v>25569.00238266019</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B96" s="4">
-        <v>26857.942552704491</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B97" s="4">
-        <v>24995.869450088339</v>
+        <v>26857.942552704491</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B98" s="4">
-        <v>25440.247753376243</v>
+        <v>24995.869450088339</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B99" s="4">
-        <v>25506.248844310558</v>
+        <v>25440.247753376243</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B100" s="4">
-        <v>26358.159693388694</v>
+        <v>25506.248844310558</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B101" s="4">
-        <v>25498.384207889791</v>
+        <v>26358.159693388694</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B102" s="4">
+        <v>25498.384207889791</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B102" s="4">
+      <c r="B103" s="4">
         <v>23173.869977272727</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="5"/>
-      <c r="B103" s="6"/>
-    </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="8" t="s">
+      <c r="A104" s="5"/>
+      <c r="B104" s="6"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B104" s="2">
+      <c r="B105" s="2">
         <v>24688.069582490236</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B105" s="4">
-        <v>22055.090994895891</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B106" s="4">
-        <v>21224.791361267176</v>
+        <v>22055.090994895891</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B107" s="4">
-        <v>28754.311781987919</v>
+        <v>21224.791361267176</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B108" s="4">
-        <v>26632.09036753347</v>
+        <v>28754.311781987919</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B109" s="4">
-        <v>23824.701185007209</v>
+        <v>26632.09036753347</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B110" s="4">
+        <v>23824.701185007209</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B110" s="4">
+      <c r="B111" s="4">
         <v>24872.53869842914</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="11"/>
-      <c r="B111" s="10"/>
-    </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="8" t="s">
+      <c r="A112" s="11"/>
+      <c r="B112" s="10"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B112" s="2">
+      <c r="B113" s="2">
         <v>34753.331091963366</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B113" s="4">
-        <v>34024.524138897541</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B114" s="4">
-        <v>45040.730192217532</v>
+        <v>34024.524138897541</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B115" s="4">
-        <v>40428.409853051293</v>
+        <v>45040.730192217532</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B116" s="4">
-        <v>35438.871174048836</v>
+        <v>40428.409853051293</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B117" s="4">
-        <v>28013.706874719352</v>
+        <v>35438.871174048836</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B118" s="4">
+        <v>28013.706874719352</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B118" s="4">
+      <c r="B119" s="4">
         <v>29156.115996085558</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="11"/>
-      <c r="B119" s="10"/>
-    </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="8" t="s">
+      <c r="A120" s="11"/>
+      <c r="B120" s="10"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B120" s="2">
+      <c r="B121" s="2">
         <v>36832.926280232939</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="B121" s="4">
-        <v>28196.623938505836</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B122" s="4">
-        <v>30038.955543266948</v>
+        <v>28196.623938505836</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B123" s="4">
-        <v>30421.555716709925</v>
+        <v>30038.955543266948</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B124" s="4">
-        <v>34263.241684077606</v>
+        <v>30421.555716709925</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B125" s="4">
-        <v>42449.94687985818</v>
+        <v>34263.241684077606</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B126" s="4">
-        <v>56198.189895321513</v>
+        <v>42449.94687985818</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B127" s="4">
-        <v>54247.157206375836</v>
+        <v>56198.189895321513</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B128" s="4">
-        <v>67826.149299820463</v>
+        <v>54247.157206375836</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B129" s="4">
+        <v>67826.149299820463</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B129" s="4">
+      <c r="B130" s="4">
         <v>65589.452333289999</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="5"/>
-      <c r="B130" s="6"/>
-    </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="8" t="s">
+      <c r="A131" s="5"/>
+      <c r="B131" s="6"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B131" s="2">
+      <c r="B132" s="2">
         <v>47110.262887027377</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B132" s="4">
-        <v>81736.54715849596</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B133" s="4">
-        <v>97253.642316433572</v>
+        <v>81736.54715849596</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B134" s="4">
-        <v>39790.240091819171</v>
+        <v>97253.642316433572</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B135" s="4">
-        <v>33701.43128620473</v>
+        <v>39790.240091819171</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B136" s="4">
-        <v>36691.478392605633</v>
+        <v>33701.43128620473</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B137" s="4">
+        <v>36691.478392605633</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B137" s="4">
+      <c r="B138" s="4">
         <v>55975.145579473152</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" s="11"/>
-      <c r="B138" s="10"/>
-    </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" s="8" t="s">
+      <c r="A139" s="11"/>
+      <c r="B139" s="10"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B139" s="2">
+      <c r="B140" s="2">
         <v>26599.004511609524</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B140" s="4">
-        <v>24884.414737719635</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B141" s="4">
-        <v>19587.094904064368</v>
+        <v>24884.414737719635</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B142" s="4">
-        <v>30153.30453444098</v>
+        <v>19587.094904064368</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B143" s="4">
-        <v>28416.052490963382</v>
+        <v>30153.30453444098</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B144" s="4">
+        <v>28416.052490963382</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B144" s="4">
+      <c r="B145" s="4">
         <v>28062.429956260723</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A145" s="9"/>
-      <c r="B145" s="7"/>
-    </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" s="8" t="s">
+      <c r="A146" s="9"/>
+      <c r="B146" s="7"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B146" s="2">
+      <c r="B147" s="2">
         <v>30169.506590296147</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="B147" s="4">
-        <v>28357.195238000593</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B148" s="4">
+        <v>28357.195238000593</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B148" s="4">
+      <c r="B149" s="4">
         <v>36426.582003659656</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A149" s="11"/>
-      <c r="B149" s="10"/>
-    </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A150" s="8" t="s">
+      <c r="A150" s="11"/>
+      <c r="B150" s="10"/>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="B150" s="2">
+      <c r="B151" s="2">
         <v>31465.850272117048</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A151" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="B151" s="4">
-        <v>34498.344995229811</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B152" s="4">
+        <v>34498.344995229811</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B152" s="4">
+      <c r="B153" s="4">
         <v>23812.022584985833</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A153" s="5"/>
-      <c r="B153" s="6"/>
-    </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" s="8" t="s">
+      <c r="A154" s="5"/>
+      <c r="B154" s="6"/>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B154" s="2">
+      <c r="B155" s="2">
         <v>34494.485931823707</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B155" s="4">
-        <v>31368.082104293884</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B156" s="4">
-        <v>23534.745027670171</v>
+        <v>31368.082104293884</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B157" s="4">
-        <v>21841.988840086608</v>
+        <v>23534.745027670171</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B158" s="4">
-        <v>28111.351410726566</v>
+        <v>21841.988840086608</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B159" s="4">
-        <v>43369.468554283601</v>
+        <v>28111.351410726566</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B160" s="4">
-        <v>38202.727063900413</v>
+        <v>43369.468554283601</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B161" s="4">
-        <v>31306.00894479451</v>
+        <v>38202.727063900413</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B162" s="4">
+        <v>31306.00894479451</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="B162" s="4">
+      <c r="B163" s="4">
         <v>54441.104586305271</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" s="11"/>
-      <c r="B163" s="10"/>
-    </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" s="8" t="s">
+      <c r="A164" s="11"/>
+      <c r="B164" s="10"/>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B164" s="2">
+      <c r="B165" s="2">
         <v>46347.008255684152</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A165" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="B165" s="4">
-        <v>52281.190739049795</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B166" s="4">
-        <v>24254.314661654134</v>
+        <v>52281.190739049795</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B167" s="4">
-        <v>29450.042165929957</v>
+        <v>24254.314661654134</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B168" s="4">
-        <v>40271.041996996995</v>
+        <v>29450.042165929957</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B169" s="4">
+        <v>40271.041996996995</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B169" s="4">
+      <c r="B170" s="4">
         <v>65879.163713692949</v>
       </c>
     </row>

</xml_diff>